<commit_message>
Agrego horas de estudio, desplazamiento y trabajo
</commit_message>
<xml_diff>
--- a/Me_programo.xlsx
+++ b/Me_programo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d02818d77b571315/Documents/universidad/2023-1/Info 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d02818d77b571315/Documents/universidad/2023-1/Info 2/programacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB532085-20DC-444E-AE7F-21B821FBA35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{EB532085-20DC-444E-AE7F-21B821FBA35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1422F98-116C-40A7-8BDC-D57262B39D32}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{20CC1194-49FF-426C-87E9-2A05042F1E1E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="27">
   <si>
     <t xml:space="preserve">Lunes </t>
   </si>
@@ -93,6 +93,30 @@
   </si>
   <si>
     <t>VIAJE A LA U</t>
+  </si>
+  <si>
+    <t>EST.PDS</t>
+  </si>
+  <si>
+    <t>EST.INFOII</t>
+  </si>
+  <si>
+    <t>EST.ROBOTICA</t>
+  </si>
+  <si>
+    <t>EST INFOII</t>
+  </si>
+  <si>
+    <t>EST INGLES</t>
+  </si>
+  <si>
+    <t>TRABAJO</t>
+  </si>
+  <si>
+    <t>EST. InGLES</t>
+  </si>
+  <si>
+    <t>VIAJE AL TRABAJO</t>
   </si>
 </sst>
 </file>
@@ -470,15 +494,17 @@
   <dimension ref="A2:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -549,7 +575,9 @@
       <c r="A5" s="2">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
@@ -562,14 +590,18 @@
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>0.375</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
@@ -582,8 +614,12 @@
       <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -602,8 +638,12 @@
       <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -622,14 +662,18 @@
       <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>0.5</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -638,19 +682,25 @@
       <c r="F9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -670,8 +720,12 @@
       <c r="F11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -690,8 +744,12 @@
       <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -712,8 +770,12 @@
       <c r="F13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -734,8 +796,12 @@
       <c r="F14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -750,34 +816,60 @@
         <v>17</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>0.83333333333333404</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -786,10 +878,16 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -798,10 +896,16 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">

</xml_diff>

<commit_message>
Asigno colores poara facilitar lectura
</commit_message>
<xml_diff>
--- a/Me_programo.xlsx
+++ b/Me_programo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d02818d77b571315/Documents/universidad/2023-1/Info 2/programacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{EB532085-20DC-444E-AE7F-21B821FBA35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1422F98-116C-40A7-8BDC-D57262B39D32}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{EB532085-20DC-444E-AE7F-21B821FBA35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0BA7894-2917-4A63-A79E-965651D6EA34}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{20CC1194-49FF-426C-87E9-2A05042F1E1E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="29">
   <si>
     <t xml:space="preserve">Lunes </t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>VIAJE AL TRABAJO</t>
+  </si>
+  <si>
+    <t>Estudio en la universidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estudio fuera de clase </t>
   </si>
 </sst>
 </file>
@@ -138,12 +144,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -173,10 +191,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -192,6 +214,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -491,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9806A62-346F-4088-BEB4-E3D21D427A42}">
-  <dimension ref="A2:H20"/>
+  <dimension ref="A2:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,9 +531,11 @@
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" customWidth="1"/>
+    <col min="12" max="12" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -531,18 +559,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0.25</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -551,18 +579,18 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.29166666666666669</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -571,23 +599,23 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -595,91 +623,99 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>0.375</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>0.41666666666666702</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>0.45833333333333298</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>0.5</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -687,11 +723,11 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="1"/>
@@ -703,21 +739,21 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>0.58333333333333304</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -727,21 +763,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>0.625</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -751,23 +787,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>0.66666666666666696</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="6" t="s">
         <v>17</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -777,23 +813,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>0.70833333333333404</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="6" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -803,16 +839,16 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>0.75</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="1"/>
@@ -823,23 +859,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -853,15 +889,15 @@
       <c r="A17" s="2">
         <v>0.83333333333333404</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -878,7 +914,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="1"/>
@@ -896,7 +932,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F19" s="1"/>

</xml_diff>